<commit_message>
"API works, schweet, pt2"
</commit_message>
<xml_diff>
--- a/data/tickerblock.xlsx
+++ b/data/tickerblock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moneybag Mike\Desktop\Fintech540-Group_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6382191A-911F-4515-904A-DAD605553227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D800A43E-223F-486F-97C1-684216CE9815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="84440" yWindow="1980" windowWidth="28800" windowHeight="15460" xr2:uid="{EEE9CE3A-66FE-4A50-A48B-CB625FBF56BA}"/>
   </bookViews>
@@ -36,23 +36,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>AMZN</t>
   </si>
   <si>
-    <t>FB</t>
-  </si>
-  <si>
     <t>RIOT</t>
   </si>
   <si>
     <t>TSLA</t>
   </si>
   <si>
-    <t>BA</t>
-  </si>
-  <si>
     <t>PLTR</t>
   </si>
   <si>
@@ -65,10 +59,49 @@
     <t>BBBY</t>
   </si>
   <si>
-    <t>COIN</t>
-  </si>
-  <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>SPCE</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>SNAP</t>
+  </si>
+  <si>
+    <t>NFLX</t>
+  </si>
+  <si>
+    <t>NVDA</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>SPOT</t>
+  </si>
+  <si>
+    <t>MSTR</t>
+  </si>
+  <si>
+    <t>SNOW</t>
+  </si>
+  <si>
+    <t>SQ</t>
+  </si>
+  <si>
+    <t>ROKU</t>
+  </si>
+  <si>
+    <t>ZM</t>
+  </si>
+  <si>
+    <t>SHOP</t>
+  </si>
+  <si>
+    <t>GOOG</t>
   </si>
 </sst>
 </file>
@@ -420,15 +453,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8977B4A1-5699-412E-8F42-BEF5BE03670C}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -440,25 +475,58 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Mike coding while frustrated..."
</commit_message>
<xml_diff>
--- a/data/tickerblock.xlsx
+++ b/data/tickerblock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moneybag Mike\Desktop\Fintech540-Group_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D800A43E-223F-486F-97C1-684216CE9815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5737090-1A96-49E8-B7EE-69660C7734BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="84440" yWindow="1980" windowWidth="28800" windowHeight="15460" xr2:uid="{EEE9CE3A-66FE-4A50-A48B-CB625FBF56BA}"/>
   </bookViews>
@@ -59,9 +59,6 @@
     <t>BBBY</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>SPCE</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>GOOG</t>
+  </si>
+  <si>
+    <t>Symbol</t>
   </si>
 </sst>
 </file>
@@ -453,80 +453,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8977B4A1-5699-412E-8F42-BEF5BE03670C}">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>